<commit_message>
Creating Main and sorting stuff out
</commit_message>
<xml_diff>
--- a/nintendo_switch_reviews.xlsx
+++ b/nintendo_switch_reviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/wrightc23_cardiff_ac_uk/Documents/Desktop University Items/Hackathons/NLP-Team1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1C0F01BDE7D3DFB10A753B5945BFB698B50E4642" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E999CF33-DC41-4236-B140-2DC5BCC4EE3B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_7D332A7DE1F4B5CBA2173C5945469E87D8C72EE6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reviews" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="215">
   <si>
     <t>id</t>
   </si>
@@ -220,6 +220,399 @@
     <t>["No Nintendo Switch 2 consoles and review samples were sent in advance, we received Nintendo's newest flagship on release day."]</t>
   </si>
   <si>
+    <t>DL-cce7387fccad72acd7b577de07a1a6e3</t>
+  </si>
+  <si>
+    <t>Nintendo Switch 2 unboxing: What do you get with the console?</t>
+  </si>
+  <si>
+    <t>https://www.indy100.com/gaming/nintendo-switch-2-unboxing-console-2672317405</t>
+  </si>
+  <si>
+    <t>Nintendo has sent review units out to media outlets for them to check out the new console and games running on it. The first thing that will be seen when unboxing are the two new Joy-Con controllers and main part of the console with the bigger screen. Below that on the next layer down is a brief user manual, a HDMI cable to connect the dock to a TV and the wrist strap accessories that connect to the Switch 2.</t>
+  </si>
+  <si>
+    <t>2025-06-05T15:19:37</t>
+  </si>
+  <si>
+    <t>['Nintendo has sent Switch 2 review units out to media outlets for them to check out the new console and games running on it.\nindy100 is very fortunate to have been sent one of these units and this is what comes in the box - read our first impressions of']</t>
+  </si>
+  <si>
+    <t>DL-0aac9eb3cc370dc0acf115375a664310</t>
+  </si>
+  <si>
+    <t>Nintendo Switch 2 launch day build-up live: all the latest news, updates, and our thoughts ahead of the console's release</t>
+  </si>
+  <si>
+    <t>https://www.techradar.com/news/live/nintendo-switch-2-launch-day-build-up-review-in-progress-live</t>
+  </si>
+  <si>
+    <t>TechRadar Gaming has been covering huge console and game launches for years - everything from reviews of Nintendo, PlayStation, and Xbox systems to key live events like Nintendo Direct and Summer Game Fest presentations. Here's a quick glance at all the Nintendo Switch 2 launch games you can expect to purchase and play on June 5.</t>
+  </si>
+  <si>
+    <t>2025-06-04T12:00:34</t>
+  </si>
+  <si>
+    <t>['Like a kid on Christmas Eve, this final day before the Nintendo Switch 2 launch may feel as long as the time between now and its official announcement way back in January. But that’s why we’re here.', 'At TechRadar Gaming, we’ve been covering huge console and game launches for years - everything from reviews of Nintendo, PlayStation, and Xbox systems to key live events like Nintendo Direct and Summer Game Fest presentations.', 'On that note, we’re confident we’ll be able to provide an interesting and informative live run-up to the Switch 2’s launch.']</t>
+  </si>
+  <si>
+    <t>DL-be4b0877ab72d480615d2f3254053e13</t>
+  </si>
+  <si>
+    <t>Moving my self-hosted empire to Proxmox was a breeze</t>
+  </si>
+  <si>
+    <t>https://www.xda-developers.com/thread/moving-my/</t>
+  </si>
+  <si>
+    <t>Nintendo has been making a lot of little weird decisions with the Switch 2. It's been a long wait for a new generation of consoles since the launch of the original hardware. Fans have speculated on a successor or major upgrade to the Switch.</t>
+  </si>
+  <si>
+    <t>2025-06-04T22:16:05+00:00</t>
+  </si>
+  <si>
+    <t>["And now, that's happening again, as outlets have confirmed they won't be publishing reviews of the Switch 2 on release day due to Nintendo not providing review units this time around. But in reality, how much does it matter?", 'Switch 2 pre-orders were flying off the shelves in the US, and the extra stock available at launch is probably going to be swooped up by die hard fans.']</t>
+  </si>
+  <si>
+    <t>DL-4e81c03324a95d53e42381b1e88678bb</t>
+  </si>
+  <si>
+    <t>Trump &amp; Xi Jinping Talk: Direct Communication Achieved</t>
+  </si>
+  <si>
+    <t>https://www.archynetys.com/trump-xi-jinping-talk-direct-communication-achieved</t>
+  </si>
+  <si>
+    <t>U.S. Treasury Secretary Scott Besent said only direct communication between Xi Jinping and Donald Trump could facilitate progress in resolving tariff disputes between the two major economies. A key point of contention for china is the United States’ restrictions on the export of advanced microchips, which are crucial for the development of Artificial Intelligence.</t>
+  </si>
+  <si>
+    <t>2025-06-06T00:07:00+00:00</t>
+  </si>
+  <si>
+    <t>['Specific Instructions\n\n   🔶 SITENAME: IGN\n   🔶 CANONICALURL:    🔶 ARTICLETITLE: Best Nintendo switch Controllers\n   🔶 METADESCRIPTION: "Looking for the best Nintendo Switch controller?', "We've tested and reviewed the top options for comfort, features, and performance.", 'SEO Optimization:\n       Incorporate the target keyword ("Best Nintendo Switch Controller") naturally throughout the article.\n       Use relevant synonyms and related keywords.']</t>
+  </si>
+  <si>
+    <t>DL-6d0e71949253ac54c4daa072e2911a23</t>
+  </si>
+  <si>
+    <t>Fortnite Nintendo Switch 2 has no 120fps mode on launch, but it’s a massive improvement over the rancid Switch 1 port</t>
+  </si>
+  <si>
+    <t>https://www.videogamer.com/news/fortnite-nintendo-switch-2-no-120fps-mode-launch/</t>
+  </si>
+  <si>
+    <t>Epic Games has released the full list of features for the Nintendo Switch 2 Edition of its free-to-play battle royale game. Fortnite runs at 60fps in both docked and handheld play, which is heaps better than the original handheld. The new handheld has higher-quality asseta across the board with textures on-par with other costumes, actual shadows and water shaders.</t>
+  </si>
+  <si>
+    <t>2025-06-04T14:57:18+00:00</t>
+  </si>
+  <si>
+    <t>["Our team of gaming experts spend hours testing and reviewing the latest games, to ensure you're reading the most comprehensive guide possible. Rest assured, all imagery and advice is unique and original.", 'Check out how we test and review games here\nEpic Games has released the full list of features for the Nintendo Switch 2 Edition of its free-to-play battle royale game.']</t>
+  </si>
+  <si>
+    <t>DL-ce5f9cdf63998a111dd0a2e7410853d6</t>
+  </si>
+  <si>
+    <t>Meta in talks with Disney, A24 and others to secure content for VR headsets</t>
+  </si>
+  <si>
+    <t>https://gigazine.net/gsc_news/en/20250605-meta-vr-contents-from-disney-a24/</t>
+  </si>
+  <si>
+    <t>FFmpeg has integrated WebRTC support, enabling ultra-low latency streaming of less than 1 second with OBS, the latest codecs can be selected, and even streaming without a server is now possible X files lawsuit against eight users who tried to unfairly increase their revenue by abusing 'creator revenue sharing' Meta announces details of AI smart glasses 'Aria Gen 2', explaining cutting-edge camera and sensor technology Results of 'MLPerf Training v5.0', which</t>
+  </si>
+  <si>
+    <t>2025-06-05T06:24:00+00:00</t>
+  </si>
+  <si>
+    <t>["reaffirms plans to invest $100 billion in Arizona over next five years\nPart of 'MetaHuman', a game development tool that allows you to create and move ultra-realistic 3DCG characters for free, is integrated into Unreal Engine 5.6\nThe reason why the Nintendo", "Switch 2 was not loaned to the media for pre-release review was because 'important features and updates for the console' will be provided on the release date of June 5th.", "Speculation is rife that the Chinese-made high-performance AI model 'DeepSeek-R1-0528' may have been distilled using Google's AI 'Gemini'\nAttention is drawn to the warning in the Nintendo Switch 2 manual that reads, 'Do not remove the shatterproof film"]</t>
+  </si>
+  <si>
+    <t>DL-0baa3766bc883eba68c2dbbae1038cce</t>
+  </si>
+  <si>
+    <t>Donkey Kong Bananza: Release date, trailer and highlights</t>
+  </si>
+  <si>
+    <t>https://www.netcost-security.fr/mobilite/252228/donkey-kong-bananza-date-de-sortie-bande-annonce-et-exclusivites-eclairantes/</t>
+  </si>
+  <si>
+    <t>The Nintendo Switch 2 is now available with an exciting set of new games. Donkey Kong Bonanza is a must-see for fans of the iconic character. Discover key details, including the release date and pre-command options.</t>
+  </si>
+  <si>
+    <t>2025-06-06T16:22:33+00:00</t>
+  </si>
+  <si>
+    <t>['To make the Switch 2 more attractive, Nintendo has released a number of games compatible only with this console. One of the games in question is a new title with Donkey Kong.', 'We will review the details of the new game, the release date of Donkey Kong Bonanza, the price, the pre-order options and the gameplay. Note that this game is only available for the Nintendo Switch 2.']</t>
+  </si>
+  <si>
+    <t>DL-48f470a3b04e45099a9bd8f8b9d0942b</t>
+  </si>
+  <si>
+    <t>What comes in the box of the Nintendo Switch 2? Look at the unboxing of the console, the Pro Controller and the camera.</t>
+  </si>
+  <si>
+    <t>https://www.tecmundo.com.br/voxel/501558-o-que-vem-na-caixa-do-nintendo-switch-2-confira-unboxing-do-console-pro-controller-e-camera.htm</t>
+  </si>
+  <si>
+    <t>Derek Keller introduces the new model of the Big N, which brings a series of innovations over the first Switch. The new model accompanies the game Mario Kart World, one of the launch titles of the new console. In addition to highlighting the visual and functional changes, the video also reveals technical details and curiosities about the accessories.</t>
+  </si>
+  <si>
+    <t>2025-06-05T21:33:00+00:00</t>
+  </si>
+  <si>
+    <t>["More compact box and redesigned design One of the first noticeable changes on the Nintendo Switch 2 is the new packaging format. Even though it's a physically larger console, the box has been optimized and it's more compact and organized.", "See this photo on Instagram A post shared by Voxel (@voxelofficial) Full review coming soon So far, Voxel has only shared the initial printouts and hardware details of Switch 2, but it's got a lot more content coming.", 'The full review of the console, the Mario Kart World, the Nintendo Camera and the new Pro Controller is already in production and should be released in the next few days. New Nintendo console in the area? Use the KaBuM dome!']</t>
+  </si>
+  <si>
+    <t>DL-7fdb288e26fb545394f161b0835d8979</t>
+  </si>
+  <si>
+    <t>Nintendo Switch 2 with Mario Kart World : Here’s how to make it cheaper with the return of your old Switch!</t>
+  </si>
+  <si>
+    <t>https://www.phonandroid.com/nintendo-switch-2-avec-mario-kart-world-voici-comment-lavoir-moins-chere-avec-la-reprise-de-votre-ancienne-switch.html</t>
+  </si>
+  <si>
+    <t>Switch 2 + Mario Kart World is available at Darty at €499.99. You can save up to €133.20 by recycling your old Switch. The Switch 2 is a new pillar of the franchise. It introduces an open world linking all circuits and 24-player races.</t>
+  </si>
+  <si>
+    <t>2025-06-07T05:00:34+00:00</t>
+  </si>
+  <si>
+    <t>['A thoroughly reviewed console and an unprecedented Mario Kart The Nintendo Switch 2 marks a real evolution from the original model.']</t>
+  </si>
+  <si>
+    <t>DL-2e469f3f8789d2c101197abc3c31aac9</t>
+  </si>
+  <si>
+    <t>Mario Kart World review – the final verdict on the Switch 2’s biggest game</t>
+  </si>
+  <si>
+    <t>https://metro.co.uk/2025/06/10/mario-kart-world-review-final-verdict-switch-2s-biggest-game-23373706/</t>
+  </si>
+  <si>
+    <t>Mario Kart 8 Deluxe is one of the very few games we’ve ever given a 10/10 score. That’s not something we regret either, especially after the extremely generous Booster Course DLC. The idea of making the next game an open world title seemed an excellent new direction to take the series. It’s very poorly utilised, with lots of hidden secrets and yet nothing of substance to gain from them.</t>
+  </si>
+  <si>
+    <t>2025-06-10T08:07:26+00:00</t>
+  </si>
+  <si>
+    <t>['Thanks to Nintendo not sending out review units of the Nintendo Switch 2 more than a day before launch we’ve previously only been able to do a review in progress of World, during which it became clear that it is not quite the game that many imagined.']</t>
+  </si>
+  <si>
+    <t>DL-4de785c3d00dac3779286d8e34763c81</t>
+  </si>
+  <si>
+    <t>How to Transfer Your Switch Data to Nintendo Switch 2</t>
+  </si>
+  <si>
+    <t>https://www.iphoneincanada.ca/2025/06/05/how-to-transfer-your-data-nintendo-switch-2/</t>
+  </si>
+  <si>
+    <t>Nintendo provides a streamlined way to conduct a system transfer from Nintendo Switch to the Switch 2. Players can transfer profile data, save data, screenshots or video, and system settings. Nintendo notes that there is an expiry date for all system transfer data.</t>
+  </si>
+  <si>
+    <t>2025-06-05T11:06:10+00:00</t>
+  </si>
+  <si>
+    <t>['By selecting ‘ I Don’t Have a Nintendo Switch 2 Yet’, you can upload your data to Nintendo’s servers in anticipation of when your Nintendo Switch 2 arrives.', 'Once the upload is complete, you can review the system transfer information and select ‘Start Restoring Factory Settings’ to complete the process. Note: This will delete all data from the original console.', 'System transfers will retain Nintendo Switch data until it’s retrieved by you on your Nintendo Switch 2. It can be restored on an original Nintendo Switch if you wish.']</t>
+  </si>
+  <si>
+    <t>DL-c52009334545d09049979dae231d50d4</t>
+  </si>
+  <si>
+    <t>How to get a Nintendo Switch 2 from Best Buy, GameStop, Target and more</t>
+  </si>
+  <si>
+    <t>https://www.independent.co.uk/extras/indybest/us/nintendo-switch-2-gamestop-best-buy-target-b2762563.html</t>
+  </si>
+  <si>
+    <t>Your support helps us to tell the story Read more Support Now From reproductive rights to Big Tech, The Independent is on the ground when the story is developing. Your donation allows us to keep sending journalists to both sides of the story. We believe quality journalism should be available to everyone, paid for by those who can afford it.</t>
+  </si>
+  <si>
+    <t>2025-06-03T10:15:58</t>
+  </si>
+  <si>
+    <t>['We got a first look at the Nintendo Switch 2 – read our hands-on review']</t>
+  </si>
+  <si>
+    <t>DL-f9f1d75efdf770e886f40ffeb4934cef</t>
+  </si>
+  <si>
+    <t>Switch 2 : the problems of Joy-Con Drift back on the new Nintendo console?</t>
+  </si>
+  <si>
+    <t>https://www.gamekult.com/actualite/switch-2-les-problemes-de-joy-con-drift-de-retour-sur-la-nouvelle-console-de-nintendo-3050864094.html</t>
+  </si>
+  <si>
+    <t>The Joy-Con Drift causes a phantom shift of the analog stick, making most games unplayable. Since 2021, more than 25,000 European complaints have led the BEUC to sue Brussels for planned obsolescence. The arrival of Switch 2, marketed on June 5, 2025, was thus seen as the final review of an industrial promise.</t>
+  </si>
+  <si>
+    <t>['Nintendo had responded with free "lifetime" repairs, but without reviewing the basic design. The arrival of Switch 2, marketed on June 5, 2025, was thus seen as the final review of an industrial promise: repairing the past to reassure the future.']</t>
+  </si>
+  <si>
+    <t>DL-1f7196f9804c69956dd1ea78f94a50cf</t>
+  </si>
+  <si>
+    <t>Switch 2: Why Nintendo doesn't want you to remove the display slide</t>
+  </si>
+  <si>
+    <t>https://t3n.de/news/switch-2-nintendo-display-folie-1691041/</t>
+  </si>
+  <si>
+    <t>On June 5, 2025, the new Nintendo console Switch 2 will officially go on sale. Pre-ordering is currently not possible on major online trading platforms. It is currently unknown when the console will be available again. Nintendo explicitly warns against removing the factory-mounted display slide.</t>
+  </si>
+  <si>
+    <t>2025-06-04T11:45:37</t>
+  </si>
+  <si>
+    <t>['Switch 2 is supposed to get new charging mode Nintendo is supposed to have found a solution for this with the Switch 2 – namely a battery-saving charging mode as usual with smartphones.', "Users should be able to set the battery to stop charging at about 90 percent capacity. View 8 images This retro technology has collector's value today Source: More on this topic MIT Technology Review Nintendo"]</t>
+  </si>
+  <si>
+    <t>DL-bc097bf1484dc8cb970325f8ea1be195</t>
+  </si>
+  <si>
+    <t>Roman Sands RE:Build release date revealed</t>
+  </si>
+  <si>
+    <t>https://www.devx.com/daily-news/roman-sands-rebuild-release-date-revealed/</t>
+  </si>
+  <si>
+    <t>Roman Sands RE:Build is coming to PS5 and PS4 on September 12th. The game focuses on providing great service and making connections with others. There are also some upcoming gaming events: The Xbox Games Showcase 2025 will feature The Outer Worlds 2 Direct on June 8 at 1:00 pm.</t>
+  </si>
+  <si>
+    <t>2025-06-09T17:16:20+00:00</t>
+  </si>
+  <si>
+    <t>['Other gaming news includes:\nReviews of how Zelda Tears of the Kingdom and Breath of the Wild run on the new Nintendo Switch 2. A look at what makes the game The Bornless different from other extraction games.']</t>
+  </si>
+  <si>
+    <t>DL-b080cb5509d88a1ec15ee8a2c6106938</t>
+  </si>
+  <si>
+    <t>Get the most out of your Nintendo Switch 2 with these 3 TVs I've picked to pair with it, including one of the best OLED TVs I've seen</t>
+  </si>
+  <si>
+    <t>https://www.techradar.com/televisions/get-the-most-out-of-your-nintendo-switch-2-with-these-3-tvs-ive-picked-to-pair-with-it-including-one-of-the-best-oled-tvs-ive-seen</t>
+  </si>
+  <si>
+    <t>TechRadar look for VRR, 120Hz refresh rate and Auto Low Latency Mode. Low input lag for responsive performance and top-notch picture quality are also important. LG B4 48-inch 4K OLED TV : £879 now £849 at Best Buy The LG C4 provides premium OLED picture quality and a full array of gaming features.</t>
+  </si>
+  <si>
+    <t>2025-06-06T08:00:00</t>
+  </si>
+  <si>
+    <t>['Plus, its rich detail and contrast are sure to give the colorful, larger-than-life graphics of the Switch 2’s games a deeper, richer look.\nThe C4’s picture quality earned 4.5 out of 5 stars in our LG C4 review for good reason!', 'And there’s no better time to buy one to pair with your Nintendo Switch 2 with ambitious ports such as Cyberpunk: 2077 available from launch.']</t>
+  </si>
+  <si>
+    <t>DL-05605b9ac8551ba2df3061a3bb23d284</t>
+  </si>
+  <si>
+    <t>My Switch 2 Review in Progress: It's Good, but Don't Give In to the FOMO Yet</t>
+  </si>
+  <si>
+    <t>https://www.cnet.com/tech/gaming/my-switch-2-review-in-progress-its-good-but-dont-give-in-to-the-fomo-yet/</t>
+  </si>
+  <si>
+    <t>The Nintendo Switch 2 is all anyone in gaming is talking about right now, and it could very well be the biggest gadget of 2025. By now, thousands of Switch 2 owners have one in hand as well, and the company will certainly sell thousands more this year. This clearly feels like a really good upgrade to aging Switches, but it's also not anything any current Switch owner needs to rush into.</t>
+  </si>
+  <si>
+    <t>2025-06-06T22:34:00+00:00</t>
+  </si>
+  <si>
+    <t>["By now, thousands of Switch 2 owners have one in hand as well, and the company will certainly sell thousands more this year, especially during the holidays. So, how good is Nintendo's new console? And is it worth upgrading from the original Switch?", "I haven't had enough time to fully review the Switch 2 yet, and the Switch 2 hasn't had enough time to spread its wings and grow its game library. These are early days for Nintendo's new console, but there's some stuff I can already tell you."]</t>
+  </si>
+  <si>
+    <t>DL-4a140a18c5aefde1b5970f7608d46b27</t>
+  </si>
+  <si>
+    <t>Nintendo Switch 2: Live updates on launch night</t>
+  </si>
+  <si>
+    <t>https://www.independent.co.uk/extras/indybest/gadgets-tech/video-games-consoles/nintendo-switch-2-stock-live-uk-b2763929.html</t>
+  </si>
+  <si>
+    <t>Smyths Toys opened all of its shops at midnight, offering a limited amount of walk-in stoc, but doors are closing at 12.30am. Over on Oxford Street, Currys is running a launch event at its flagship store. A few retailers are holding back stock for the early hours of the morning. Retailers are gearing up to drop more Switch 2 stock online as the morning unfolds.</t>
+  </si>
+  <si>
+    <t>2025-06-04T21:52:05+00:00</t>
+  </si>
+  <si>
+    <t>['Oh, and there will be limited stock of the Nintendo Switch 2 available, too.', 'Alex Lee4 June 2025 22:00\n2 hours ago\nMario Kart World review\nTech writer Steve Hogarty spent six hours playing Mario Kart World – and he certainly had some thoughts (19 in fact).']</t>
+  </si>
+  <si>
+    <t>DL-8eed788f4c6b98f895779a24abd5aba6</t>
+  </si>
+  <si>
+    <t>Nintendo Switch 2 guide: pre-order links, accessories and launch games</t>
+  </si>
+  <si>
+    <t>https://www.theshortcut.com/p/nintendo-switch-2-guide-pre-order-live</t>
+  </si>
+  <si>
+    <t>There are 10 tech stories in today’s Substack issue of The Shortcut Skip ahead to story 2 to 10 for more Nintendo Switch 2 is arriving at stores across the United States tonight. This is your chance to skip the line. Walmart always has more console inventory and better servers than GameStop.</t>
+  </si>
+  <si>
+    <t>2025-06-05T03:05:04</t>
+  </si>
+  <si>
+    <t>['My personal Switch 2 pre-order from Target was delayed at the last minute. So I’m in line – with the diehard Nintendo gamers, some of whom arrived at 8am ET – hoping to secure a Switch 2 from Best Buy at midnight. Review coming soon.\nThe best part?']</t>
+  </si>
+  <si>
+    <t>DL-fb44e9ba1c36059416a5f81b3d4717bc</t>
+  </si>
+  <si>
+    <t>Nintendo Switch 2 is here - first impressions</t>
+  </si>
+  <si>
+    <t>https://www.gram.pl/artykul/nintendo-switch-2-juz-tu-jest-pierwsze-wrazenia</t>
+  </si>
+  <si>
+    <t>Nintendo Switch 2 is one of my favorite consoles, which has accompanied me in various roles for over eight years. The first Switch was with me until the release of the OLED version in 2021. I forgave myself for Lite, because it did not correspond to my preferences of playing mainly on TV.</t>
+  </si>
+  <si>
+    <t>2025-06-07T19:00:00</t>
+  </si>
+  <si>
+    <t>['But when the long-awaited Switch 2 appeared on the horizon, placing a pre-release order was obvious.', 'I will immediately point out that this text is not a racial review of the equipment, but rather an impression, a collection of first impressions and thoughts about the new Nintendo toy.', 'Nintendo Switch 2 is a console that can be labeled the “new generation”, and at the same time it is very strongly rooted in what the first Switch accustomed us to. More a subdued but significant evolution than a surprising revolution.']</t>
+  </si>
+  <si>
+    <t>DL-52361e315938e25ca5f998c23b324103</t>
+  </si>
+  <si>
+    <t>Nintendo Switch 2: Should I buy it now or wait?</t>
+  </si>
+  <si>
+    <t>https://www.presse-citron.net/nintendo-switch-2-faut-il-lacheter-maintenant-ou-attendre/</t>
+  </si>
+  <si>
+    <t>Nintendo is changing its habits with the Switch 2. For the first time in years, the Kyoto firm did not send its console to journalists several weeks before the launch. As a result, in-depth testing will arrive after the sale, leaving some players in uncertainty.</t>
+  </si>
+  <si>
+    <t>2025-06-05T10:19:31+00:00</t>
+  </si>
+  <si>
+    <t>['So, are we buying Switch 2 today or not? The decision ultimately depends on your player profile and your priorities. The unconditional Nintendo fans and early adopters assumed will in any case dark without remorse.', 'I think the more measured players will benefit from waiting for our full review next week by identifying the console’s strengths and weaknesses, and then being able to make a fully informed choice.']</t>
+  </si>
+  <si>
+    <t>DL-c7d6e0b0219f3beca439c15760b9c7ab</t>
+  </si>
+  <si>
+    <t>A look at Nintendo Switch 2</t>
+  </si>
+  <si>
+    <t>https://nintendon.it/2025/06/05/un-primo-sguardo-a-nintendo-switch-2-312815</t>
+  </si>
+  <si>
+    <t>Nintendo released the spiritual and conceptual successor to one of the most successful consoles of all time, the Nintendo Switch. The concept of hybrid consoles has had such an impact on the market that it has created a line of consoles that are now continuing their quest for technological evolution. We're talking about almost one inch more screen than the original Joycon, which was smaller and often annoying in the short run.</t>
+  </si>
+  <si>
+    <t>2025-06-05T18:31:57+00:00</t>
+  </si>
+  <si>
+    <t>['This is something that will surely be wiped out over the years, of the reviews and pieces that each and every one of us will write from here over the next few years on the site.', "But there's certainly a huge difference immediately between the games that were designed for the Nintendo Switch and the ones that are coming in natively on the Nintendo Switch 2."]</t>
+  </si>
+  <si>
     <t>query_text</t>
   </si>
   <si>
@@ -262,7 +655,7 @@
     <t>source_document_ids</t>
   </si>
   <si>
-    <t>Current reviews on the Nintendo Switch 2 are limited as there were no pre-launch review units provided to the press, with reports indicating that reviews would be available after the launch on June 5, 2025. Early impressions suggest that the console became available in stores on June 6, 2025, and initial access has been positive, with reviewers starting to share their thoughts. For example, an early review notes that many were surprised to find the console available in retail stores after pre-orders. However, comprehensive reviews are still pending as of now. [Nintendo confirms no Switch 2 reviews ahead of launch](https://mobilesyrup.com/2025/06/03/nintendo-confirms-no-switch-2-reviews/), [Nintendo Switch 2: Early review thoughts from our first days with the gaming system](https://www.engadget.com/gaming/nintendo/nintendo-switch-2-early-review-thoughts-from-our-first-days-with-the-gaming-system-143545893.html).</t>
+    <t>Current reviews on the Nintendo Switch 2 are limited as there were no pre-launch review units provided to the press, with reports indicating that reviews would be available after the launch on June 5, 2025. Early impressions suggest that the console became available in stores on June 6, 2025, and initial access has been positive for those who pre-ordered or purchased it in retail stores. A full review is expected to be published soon. For more details, see [Nintendo confirms no Switch 2 reviews ahead of launch](https://mobilesyrup.com/2025/06/03/nintendo-confirms-no-switch-2-reviews/), [Nintendo Switch 2: Early review thoughts from our first days with the gaming system](https://www.engadget.com/gaming/nintendo/nintendo-switch-2-early-review-thoughts-from-our-first-days-with-the-gaming-system-143545893.html).</t>
   </si>
   <si>
     <t>['DL-5ac62016344eb6e53697f78afd2d87ac', 'DL-56b3456fa4d4c2c0316f8c748ec38942', 'DL-2a418e6f75f602bcd521348ca4edc33a', 'DL-251c66dcd4b421aa53f620b9134f31c2', 'DL-5513a1a5febbfb007ca5e4787a99aac2']</t>
@@ -281,7 +674,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,14 +686,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -335,19 +720,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -648,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,7 +1075,7 @@
         <v>10</v>
       </c>
       <c r="E2">
-        <v>182.02428</v>
+        <v>182.02739</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -713,7 +1095,7 @@
         <v>15</v>
       </c>
       <c r="E3">
-        <v>104.13048999999999</v>
+        <v>104.14435</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -736,7 +1118,7 @@
         <v>21</v>
       </c>
       <c r="E4">
-        <v>93.144679999999994</v>
+        <v>93.145979999999994</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>
@@ -759,7 +1141,7 @@
         <v>27</v>
       </c>
       <c r="E5">
-        <v>91.555189999999996</v>
+        <v>91.555220000000006</v>
       </c>
       <c r="F5" t="s">
         <v>28</v>
@@ -782,7 +1164,7 @@
         <v>33</v>
       </c>
       <c r="E6">
-        <v>75.955475000000007</v>
+        <v>75.957183999999998</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
@@ -805,7 +1187,7 @@
         <v>38</v>
       </c>
       <c r="E7">
-        <v>69.502494999999996</v>
+        <v>69.451700000000002</v>
       </c>
       <c r="F7" t="s">
         <v>39</v>
@@ -828,7 +1210,7 @@
         <v>44</v>
       </c>
       <c r="E8">
-        <v>26.114891</v>
+        <v>26.115057</v>
       </c>
       <c r="F8" t="s">
         <v>45</v>
@@ -851,7 +1233,7 @@
         <v>50</v>
       </c>
       <c r="E9">
-        <v>15.326954000000001</v>
+        <v>15.327070000000001</v>
       </c>
       <c r="F9" t="s">
         <v>51</v>
@@ -874,7 +1256,7 @@
         <v>56</v>
       </c>
       <c r="E10">
-        <v>10.091889999999999</v>
+        <v>10.091949</v>
       </c>
       <c r="F10" t="s">
         <v>57</v>
@@ -890,14 +1272,14 @@
       <c r="B11" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>61</v>
       </c>
       <c r="D11" t="s">
         <v>62</v>
       </c>
       <c r="E11">
-        <v>9.9057879999999994</v>
+        <v>9.9058060000000001</v>
       </c>
       <c r="F11" t="s">
         <v>63</v>
@@ -906,10 +1288,510 @@
         <v>64</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12">
+        <v>6.5716057000000001</v>
+      </c>
+      <c r="F12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13">
+        <v>5.8586939999999998</v>
+      </c>
+      <c r="F13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14">
+        <v>4.3080882999999996</v>
+      </c>
+      <c r="F14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15">
+        <v>4.1230792999999997</v>
+      </c>
+      <c r="F15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16">
+        <v>3.2429503999999998</v>
+      </c>
+      <c r="F16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17">
+        <v>2.8485813000000002</v>
+      </c>
+      <c r="F17" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18">
+        <v>2.6608944000000001</v>
+      </c>
+      <c r="F18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19">
+        <v>2.5883693999999999</v>
+      </c>
+      <c r="F19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20">
+        <v>2.2660236</v>
+      </c>
+      <c r="F20" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21">
+        <v>2.2052078000000002</v>
+      </c>
+      <c r="F21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22">
+        <v>1.8887423999999999</v>
+      </c>
+      <c r="F22" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23">
+        <v>1.8627967999999999</v>
+      </c>
+      <c r="F23" t="s">
+        <v>135</v>
+      </c>
+      <c r="G23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24" t="s">
+        <v>140</v>
+      </c>
+      <c r="E24">
+        <v>1.5330296000000001</v>
+      </c>
+      <c r="G24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" t="s">
+        <v>144</v>
+      </c>
+      <c r="D25" t="s">
+        <v>145</v>
+      </c>
+      <c r="E25">
+        <v>1.2448444000000001</v>
+      </c>
+      <c r="F25" t="s">
+        <v>146</v>
+      </c>
+      <c r="G25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D26" t="s">
+        <v>151</v>
+      </c>
+      <c r="E26">
+        <v>1.1689453000000001</v>
+      </c>
+      <c r="F26" t="s">
+        <v>152</v>
+      </c>
+      <c r="G26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E27">
+        <v>0.95645714000000004</v>
+      </c>
+      <c r="F27" t="s">
+        <v>158</v>
+      </c>
+      <c r="G27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>160</v>
+      </c>
+      <c r="B28" t="s">
+        <v>161</v>
+      </c>
+      <c r="C28" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28">
+        <v>0.64604950000000005</v>
+      </c>
+      <c r="F28" t="s">
+        <v>164</v>
+      </c>
+      <c r="G28" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" t="s">
+        <v>169</v>
+      </c>
+      <c r="E29">
+        <v>0.64416313000000003</v>
+      </c>
+      <c r="F29" t="s">
+        <v>170</v>
+      </c>
+      <c r="G29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" t="s">
+        <v>173</v>
+      </c>
+      <c r="C30" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" t="s">
+        <v>175</v>
+      </c>
+      <c r="E30">
+        <v>0.63585659999999999</v>
+      </c>
+      <c r="F30" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>178</v>
+      </c>
+      <c r="B31" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" t="s">
+        <v>180</v>
+      </c>
+      <c r="D31" t="s">
+        <v>181</v>
+      </c>
+      <c r="E31">
+        <v>0.52190020000000004</v>
+      </c>
+      <c r="F31" t="s">
+        <v>182</v>
+      </c>
+      <c r="G31" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>184</v>
+      </c>
+      <c r="B32" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" t="s">
+        <v>187</v>
+      </c>
+      <c r="E32">
+        <v>0.35094259999999999</v>
+      </c>
+      <c r="F32" t="s">
+        <v>188</v>
+      </c>
+      <c r="G32" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>190</v>
+      </c>
+      <c r="B33" t="s">
+        <v>191</v>
+      </c>
+      <c r="C33" t="s">
+        <v>192</v>
+      </c>
+      <c r="D33" t="s">
+        <v>193</v>
+      </c>
+      <c r="E33">
+        <v>0.28358270000000002</v>
+      </c>
+      <c r="F33" t="s">
+        <v>194</v>
+      </c>
+      <c r="G33" t="s">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{8BC49F9D-18C5-4E0B-87EE-476336BF4852}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -924,51 +1806,51 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>196</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>197</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>198</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>199</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>200</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>70</v>
+        <v>201</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>71</v>
+        <v>202</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>72</v>
+        <v>203</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>73</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>205</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>206</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -986,18 +1868,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>208</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -1015,24 +1897,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>212</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>213</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>